<commit_message>
clientValidation, mail and user
</commit_message>
<xml_diff>
--- a/PlanillaCorreccionPrimeraEntregaObligatorio2019.xlsx
+++ b/PlanillaCorreccionPrimeraEntregaObligatorio2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avall\Documents\Andrés\ORT\Programación 2\avallelisboa\Obligatorio1P2-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EC0EF5-694A-4842-BA17-1F11C22E3055}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5AA336-0195-4CA1-8AEC-D2D5E095D263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>Item</t>
   </si>
@@ -735,8 +735,8 @@
   </sheetPr>
   <dimension ref="A1:T239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1086,7 +1086,9 @@
       <c r="B18" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="D18" s="8"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -1110,7 +1112,9 @@
       <c r="B19" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="D19" s="8"/>
     </row>
     <row r="20" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1118,7 +1122,9 @@
       <c r="B20" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1126,21 +1132,27 @@
       <c r="B21" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="16"/>
+      <c r="C22" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="D22" s="30"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="16"/>
+      <c r="C23" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="D23" s="30"/>
     </row>
     <row r="24" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1156,7 +1168,9 @@
       <c r="B25" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="13"/>
+      <c r="C25" s="13" t="s">
+        <v>47</v>
+      </c>
       <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1164,7 +1178,9 @@
       <c r="B26" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="13"/>
+      <c r="C26" s="13" t="s">
+        <v>47</v>
+      </c>
       <c r="D26" s="8"/>
     </row>
     <row r="27" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1180,7 +1196,9 @@
       <c r="B28" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="13"/>
+      <c r="C28" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="D28" s="8"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -1204,7 +1222,9 @@
       <c r="B29" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="13"/>
+      <c r="C29" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="D29" s="8"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -1228,7 +1248,9 @@
       <c r="B30" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="13"/>
+      <c r="C30" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="D30" s="8"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -1252,7 +1274,9 @@
       <c r="B31" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="13"/>
+      <c r="C31" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="D31" s="8"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -1300,7 +1324,9 @@
       <c r="B33" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="13"/>
+      <c r="C33" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="D33" s="8"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -1324,7 +1350,9 @@
       <c r="B34" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="14"/>
+      <c r="C34" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="D34" s="8"/>
     </row>
     <row r="35" spans="1:20" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.35">
@@ -1332,7 +1360,9 @@
       <c r="B35" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="13"/>
+      <c r="C35" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="D35" s="8"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -1355,7 +1385,9 @@
       <c r="B36" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="21"/>
+      <c r="C36" s="21" t="s">
+        <v>46</v>
+      </c>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.35">
@@ -1370,7 +1402,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D38" s="1"/>
     </row>
@@ -1379,7 +1411,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D39" s="1"/>
     </row>
@@ -1388,7 +1420,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D40" s="1"/>
     </row>
@@ -1406,7 +1438,7 @@
         <v>41</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D42" s="1"/>
     </row>

</xml_diff>

<commit_message>
list clients before date
</commit_message>
<xml_diff>
--- a/PlanillaCorreccionPrimeraEntregaObligatorio2019.xlsx
+++ b/PlanillaCorreccionPrimeraEntregaObligatorio2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avall\Documents\Andrés\ORT\Programación 2\avallelisboa\Obligatorio1P2-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFAEDD3-568C-407F-ADF8-69408212C84F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B6A5CB-0AE7-4D6F-9656-A85B6B5EEE98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -739,7 +739,7 @@
   <dimension ref="A1:T239"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1200,7 +1200,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="7"/>
@@ -1252,7 +1252,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="7"/>
@@ -1278,7 +1278,7 @@
         <v>35</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="7"/>

</xml_diff>

<commit_message>
List purchases and list clients
</commit_message>
<xml_diff>
--- a/PlanillaCorreccionPrimeraEntregaObligatorio2019.xlsx
+++ b/PlanillaCorreccionPrimeraEntregaObligatorio2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avall\Documents\Andrés\ORT\Programación 2\avallelisboa\Obligatorio1P2-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B6A5CB-0AE7-4D6F-9656-A85B6B5EEE98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604BFA13-EFF0-4912-9DCC-0F9AA7D96B6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>Item</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>TF</t>
   </si>
 </sst>
 </file>
@@ -738,8 +735,8 @@
   </sheetPr>
   <dimension ref="A1:T239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1040,7 +1037,7 @@
         <v>18</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="30"/>
       <c r="E16" s="1"/>
@@ -1328,7 +1325,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="7"/>
@@ -1389,7 +1386,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D36" s="1"/>
     </row>
@@ -1432,7 +1429,7 @@
         <v>40</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D41" s="1"/>
     </row>

</xml_diff>